<commit_message>
feat: modify test case and calc format result
</commit_message>
<xml_diff>
--- a/test/data/qa.xlsx
+++ b/test/data/qa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Features\Documents\PMB-UNDIKSHA\va-pmb-undiksha\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB89B75B-CF5D-47F5-8EAF-B9D949A35525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9DD13C-154E-4817-BF5E-A15AB49BC4B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A7FD8239-2D96-4688-A048-ADBE3AAB3502}"/>
   </bookViews>
@@ -213,150 +213,190 @@
     <t>Berapa biaya mengikuti SNBT?</t>
   </si>
   <si>
-    <t>Salam Harmoni🙏
-Daya tampung mahasiswa untuk Program Studi Ilmu Komputer (S1) di Universitas Pendidikan Ganesha adalah 110 mahasiswa.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Anda dapat mendapatkan informasi mengenai fasilitas layanan konseling di Universitas Pendidikan Ganesha dengan menghubungi unit konseling yang tersedia. Layanan ini ditangani oleh konselor yang berpengalaman dan dapat membantu mahasiswa dalam memecahkan masalah akademik dan non akademik. Untuk informasi lebih lanjut, Anda dapat menghubungi nomor berikut: (+6281246318813).</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Dekan Fakultas Bahasa dan Seni (FBS) Universitas Pendidikan Ganesha adalah Drs. I Gede Nurjaya, M.Pd.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Nama dekan Fakultas Ilmu Pendidikan (FIP) Universitas Pendidikan Ganesha adalah Prof. Dr. I Wayan Widiana, S.Pd., M.Pd.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Fakultas Ilmu Pendidikan (FIP) Universitas Pendidikan Ganesha mulai berdiri pada tahun 1968. Jurusan awal yang ada di fakultas ini adalah Bimbingan dan Penyuluhan serta Pendidikan Luar Sekolah.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Fakultas Kedokteran Universitas Pendidikan Ganesha (Undiksha) didirikan berdasarkan Keputusan Menteri Riset Teknologi dan Pendidikan Tinggi Republik Indonesia, Nomor: 574/KPT/I/2018 tertanggal 16 Juli 2018.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Visi Fakultas Kedokteran (FK) Universitas Pendidikan Ganesha adalah menjadi program studi kedokteran unggul dalam bidang kedokteran pariwisata berlandaskan Falsafah Tri Hita Karana di Asia Tahun 2045.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Dekan Fakultas Matematika dan Ilmu Pengetahuan Alam (FMIPA) Universitas Pendidikan Ganesha adalah Dr. I Wayan Sukra Warpala, S.Pd., M.Sc.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Program Studi Pendidikan Olahraga dan Kesehatan pertama kali berdiri pada tahun 1988 di bawah Jurusan Pendidikan Matematika dan Ilmu Pengetahuan Alam (MIPA).</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Visi Fakultas Olahraga dan Kesehatan (FOK) Universitas Pendidikan Ganesha adalah menjadi Fakultas unggul dalam menghasilkan Sumber Daya Manusia (SDM) di bidang keolahragaan dan kesehatan berlandaskan falsafah Tri Hita Karana di Indonesia tahun 2045.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Fakultas Teknik dan Kejuruan (FTK) Universitas Pendidikan Ganesha mulai berdiri pada tahun 1990. Program studi awal yang ditawarkan adalah Pendidikan Kesejahteraan Keluarga di bawah Jurusan Ilmu Pendidikan.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Dekan Fakultas Teknik dan Kejuruan (FTK) Universitas Pendidikan Ganesha adalah Dr. Kadek Rihendra Dantes, S.T., M.T.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Kepala UPA TIK Universitas Pendidikan Ganesha saat ini adalah I Ketut Resika Arthana, S.T., M.Kom.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Motto Universitas Pendidikan Ganesha (Undiksha) adalah “dharmaning sajjana umerdhyaken widyaguna” yang berarti kewajiban orang bijaksana adalah mengembangkan ilmu pengetahuan dan pekerti.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Rektor Universitas Pendidikan Ganesha saat ini adalah Prof. Dr. I Wayan Lasmawan, M.Pd.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Anda dapat melihat KTM melalui SSO Undiksha atau dengan mengirimkan pesan yang berisi NIM (Nomor Induk Mahasiswa) yang valid. NIM yang valid dari Undiksha terdiri dari 10 digit angka. 
-Untuk mengirimkan pesan, gunakan format berikut:
-- KTM [NIM]
-Contoh penulisan pesan:
-- KTM 1234567890
-Silakan kirimkan NIM Anda untuk mendapatkan informasi lebih lanjut.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Program Adik Papua ialah program keberpihakan bagi putra-putri asli Papua di Provinsi Papua dan Provinsi Papua Barat dengan memberi kesempatan belajar di perguruan tinggi negeri yang diselenggarakan oleh Kemdikbud melalui mekanisme seleksi khusus siswa SMA sederajat, berdasarkan penjaringan prestasi akademik. Daerah yang menjadi sasaran pelaksanaan di Provinsi Papua dan Provinsi Papua Barat, meliputi; Kabupaten/Kota yang memiliki SMA sederajat dan memenuhi syarat sebagai peserta program ADik papua, sebagaimana diatur oleh Undang-Undang. Website resmi: https://adik.kemdikbud.go.id</t>
-  </si>
-  <si>
     <t>Dimana saya dapat melihat informasi daya tampung Mahasiswa Baru Undiksha Tahun Akademik 2024/2025?</t>
   </si>
   <si>
     <t>Fasilitas apa saja yang dimiliki undiksha?</t>
   </si>
   <si>
-    <t>Salam Harmoni🙏
-Visi Fakultas Matematika dan Ilmu Pengetahuan Alam (FMIPA) Universitas Pendidikan Ganesha adalah "Menjadi Fakultas Unggul Dalam Matematika Dan Ilmu Pengetahuan Alam Berlandaskan Falsafah Tri Hita Karana Di Asia Tahun 2045."</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Kurikulum dikembangkan sesuai dengan visi, misi, tujuan, dan sasaran Undiksha yang berbasis kompetensi dan berorientasi Kerangka Kualifikasi Nasional Indonesia (KKNI).</t>
-  </si>
-  <si>
     <t>Pengembangan kurikulum Undiksha sesuai dengan apa?</t>
   </si>
   <si>
     <t>Siapa nama Direktur Pascasarjana Universitas Pendidikan Ganesha?</t>
   </si>
   <si>
-    <t>Salam Harmoni🙏
-Direktur Pascasarjana Universitas Pendidikan Ganesha adalah Prof. Dr. I Nyoman Jampel, M.Pd.</t>
-  </si>
-  <si>
     <t>Sebutkan program doktoral yang ditawarkan oleh Fakultas Pascasarjana Universitas Pendidikan Ganesha.</t>
   </si>
   <si>
-    <t>Salam Harmoni🙏
-Prinsip SNPMB (Seleksi Nasional Penerimaan Mahasiswa Baru) meliputi:
-1. Fleksibel: Proses seleksi dirancang untuk memberikan kemudahan bagi peserta dalam mengikuti ujian.
-2. Efisien: Mengutamakan penggunaan sumber daya secara optimal untuk mencapai hasil yang maksimal.
-3. Transparan: Proses seleksi dilakukan secara terbuka dan dapat dipertanggungjawabkan.
-4. Adil: Memberikan kesempatan yang sama bagi semua peserta tanpa diskriminasi.
-5. Larangan Berkonflik: Menghindari adanya konflik kepentingan dalam proses seleksi.
-6. Akuntabel: Setiap tahapan dan keputusan dalam proses seleksi dapat dipertanggungjawabkan.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Biaya untuk mengikuti Seleksi Nasional Berdasarkan Tes (SNBT) adalah sebesar Rp200.000,00 (dua ratus ribu rupiah). Pembayaran dilakukan melalui mitra bank yang ditentukan.</t>
-  </si>
-  <si>
     <t>Bagaimana cara mendapat informasi lebih lanjut tentang UKM di Undiksha?</t>
   </si>
   <si>
-    <t>Salam Harmoni🙏
-Visi Universitas Pendidikan Ganesha (Undiksha) adalah menjadi Universitas Unggul Berlandaskan Falsafah Tri Hita Karana di Asia Pada Tahun 2045.</t>
-  </si>
-  <si>
     <t>Apa jenis-jenis beasiswa bagi mahasiswa undiksha?</t>
   </si>
   <si>
-    <t>Salam Harmoni🙏
-Anda dapat melihat informasi daya tampung mahasiswa baru Universitas Pendidikan Ganesha tahun akademik 2024/2025 dengan mengunjungi tautan berikut: https://undiksha.ac.id/pmb/tahun2024/daya-tampung.</t>
-  </si>
-  <si>
     <t>FHIS punya video profil?</t>
   </si>
   <si>
     <t>Coba kirimkan web FHIS</t>
   </si>
   <si>
-    <t>Salam Harmoni🙏
-Anda dapat mengunjungi website Fakultas Hukum dan Ilmu Sosial Universitas Pendidikan Ganesha (Undiksha) melalui tautan berikut: http://fhis.undiksha.ac.id</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Ya, Fakultas Hukum dan Ilmu Sosial (FHIS) Universitas Pendidikan Ganesha memiliki video profil. Anda dapat menontonnya melalui tautan berikut: https://youtu.be/xrruGWs5HNk. Video ini memberikan informasi mengenai program studi, kegiatan, dan keunggulan yang ditawarkan oleh FHIS</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Berikut informasi Kelulusan Peserta SMBJM di Undiksha (Universitas Pendidikan Ganesha):
+    <t>Apa itu Estimasi Biaya Kuliah?</t>
+  </si>
+  <si>
+    <t>Visi Fakultas Ekonomi</t>
+  </si>
+  <si>
+    <t>Kapan jadwal pendaftaran SMBJM?</t>
+  </si>
+  <si>
+    <t>Siapa nama Wakil Dekan I FE?</t>
+  </si>
+  <si>
+    <t>Siapa nama Dekan FIP?</t>
+  </si>
+  <si>
+    <t>Kapan FIP mulai berdiri dan apa jurusan awalnya?</t>
+  </si>
+  <si>
+    <t>Link informasi cara pembayaran UKT Mahasiswa Baru Undiksha dengan Layanan BRI Virtual Account (BRIVA)</t>
+  </si>
+  <si>
+    <t>Saya ingin lihat KTM, NIM saya 2115101014.</t>
+  </si>
+  <si>
+    <t>Siapa presiden indonesia sekarang?</t>
+  </si>
+  <si>
+    <t>Presiden</t>
+  </si>
+  <si>
+    <t>Berapa daya tampung mahasiswa program studi ilmu komputer S1?</t>
+  </si>
+  <si>
+    <t>Kapan FK didirikan?</t>
+  </si>
+  <si>
+    <t>Apa visi dari FK?</t>
+  </si>
+  <si>
+    <t>Apa visi dari FMIPA?</t>
+  </si>
+  <si>
+    <t>Siapa Dekan FMIPA?</t>
+  </si>
+  <si>
+    <t>Apa visi dari FOK?</t>
+  </si>
+  <si>
+    <t>Kapan FTK mulai berdiri dan program studi awal apa yang ditawarkan?</t>
+  </si>
+  <si>
+    <t>Siapa Dekan FTK?</t>
+  </si>
+  <si>
+    <t>Apa fungsi utama UKM di Universitas Pendidikan Ganesha?</t>
+  </si>
+  <si>
+    <t>Apa tugas utama dari UPA TIK?</t>
+  </si>
+  <si>
+    <t>Siapa kepala UPA TIK saat ini?</t>
+  </si>
+  <si>
+    <t>Program Adik Papua ialah program keberpihakan bagi putra-putri asli Papua di Provinsi Papua dan Provinsi Papua Barat dengan memberi kesempatan belajar di perguruan tinggi negeri yang diselenggarakan oleh Kemdikbud melalui mekanisme seleksi khusus siswa SMA sederajat, berdasarkan penjaringan prestasi akademik. Daerah yang menjadi sasaran pelaksanaan di Provinsi Papua dan Provinsi Papua Barat, meliputi; Kabupaten/Kota yang memiliki SMA sederajat dan memenuhi syarat sebagai peserta program ADik papua, sebagaimana diatur oleh Undang-Undang. Website resmi: https://adik.kemdikbud.go.id</t>
+  </si>
+  <si>
+    <t>Anda dapat melihat informasi daya tampung mahasiswa baru Universitas Pendidikan Ganesha tahun akademik 2024/2025 dengan mengunjungi tautan berikut: https://undiksha.ac.id/pmb/tahun2024/daya-tampung.</t>
+  </si>
+  <si>
+    <t>Daya tampung mahasiswa untuk Program Studi Ilmu Komputer (S1) di Universitas Pendidikan Ganesha adalah 110 mahasiswa.</t>
+  </si>
+  <si>
+    <t>Estimasi biaya kuliah adalah perkiraan biaya yang harus ditanggung oleh calon mahasiswa per semester jika mengikuti perkuliahan di Universitas Pendidikan Ganesha (Undiksha). Biaya ini mencakup berbagai komponen, seperti biaya pendidikan, biaya administrasi, dan biaya lainnya yang mungkin diperlukan selama proses perkuliahan. Estimasi ini penting untuk membantu calon mahasiswa merencanakan keuangan mereka selama menempuh pendidikan di Undiksha.</t>
+  </si>
+  <si>
+    <t>Anda dapat mendapatkan informasi mengenai fasilitas layanan konseling di Universitas Pendidikan Ganesha dengan menghubungi unit konseling yang tersedia. Layanan ini ditangani oleh konselor yang berpengalaman dan dapat membantu mahasiswa dalam memecahkan masalah akademik dan non akademik. Untuk informasi lebih lanjut, Anda dapat menghubungi nomor berikut: (+6281246318813).</t>
+  </si>
+  <si>
+    <t>Dekan Fakultas Bahasa dan Seni (FBS) Universitas Pendidikan Ganesha adalah Drs. I Gede Nurjaya, M.Pd.</t>
+  </si>
+  <si>
+    <t>Nama Wakil Dekan I Fakultas Ekonomi (FE) Universitas Pendidikan Ganesha adalah Dr. Dra. Ni Made Suci, M.Si.</t>
+  </si>
+  <si>
+    <t>Visi Fakultas Ekonomi (FE) Universitas Pendidikan Ganesha adalah "Menjadi Fakultas Unggul Berjiwa Wirausaha Berlandaskan Falsafah Tri Hita Karana di Asia Tahun 2045."</t>
+  </si>
+  <si>
+    <t>Anda dapat mengunjungi website Fakultas Hukum dan Ilmu Sosial Universitas Pendidikan Ganesha (Undiksha) melalui tautan berikut: http://fhis.undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>Ya, Fakultas Hukum dan Ilmu Sosial (FHIS) Universitas Pendidikan Ganesha memiliki video profil. Anda dapat menontonnya melalui tautan berikut: https://youtu.be/xrruGWs5HNk. Video ini memberikan informasi mengenai program studi, kegiatan, dan keunggulan yang ditawarkan oleh FHIS</t>
+  </si>
+  <si>
+    <t>Nama dekan Fakultas Ilmu Pendidikan (FIP) Universitas Pendidikan Ganesha adalah Prof. Dr. I Wayan Widiana, S.Pd., M.Pd.</t>
+  </si>
+  <si>
+    <t>Fakultas Ilmu Pendidikan (FIP) Universitas Pendidikan Ganesha mulai berdiri pada tahun 1968. Jurusan awal yang ada di fakultas ini adalah Bimbingan dan Penyuluhan serta Pendidikan Luar Sekolah.</t>
+  </si>
+  <si>
+    <t>Fakultas Kedokteran Universitas Pendidikan Ganesha (Undiksha) didirikan berdasarkan Keputusan Menteri Riset Teknologi dan Pendidikan Tinggi Republik Indonesia, Nomor: 574/KPT/I/2018 tertanggal 16 Juli 2018.</t>
+  </si>
+  <si>
+    <t>Visi Fakultas Kedokteran (FK) Universitas Pendidikan Ganesha adalah menjadi program studi kedokteran unggul dalam bidang kedokteran pariwisata berlandaskan Falsafah Tri Hita Karana di Asia Tahun 2045.</t>
+  </si>
+  <si>
+    <t>Visi Fakultas Matematika dan Ilmu Pengetahuan Alam (FMIPA) Universitas Pendidikan Ganesha adalah "Menjadi Fakultas Unggul Dalam Matematika Dan Ilmu Pengetahuan Alam Berlandaskan Falsafah Tri Hita Karana Di Asia Tahun 2045."</t>
+  </si>
+  <si>
+    <t>Dekan Fakultas Matematika dan Ilmu Pengetahuan Alam (FMIPA) Universitas Pendidikan Ganesha adalah Dr. I Wayan Sukra Warpala, S.Pd., M.Sc.</t>
+  </si>
+  <si>
+    <t>Program Studi Pendidikan Olahraga dan Kesehatan pertama kali berdiri pada tahun 1988 di bawah Jurusan Pendidikan Matematika dan Ilmu Pengetahuan Alam (MIPA).</t>
+  </si>
+  <si>
+    <t>Visi Fakultas Olahraga dan Kesehatan (FOK) Universitas Pendidikan Ganesha adalah menjadi Fakultas unggul dalam menghasilkan Sumber Daya Manusia (SDM) di bidang keolahragaan dan kesehatan berlandaskan falsafah Tri Hita Karana di Indonesia tahun 2045.</t>
+  </si>
+  <si>
+    <t>Fakultas Teknik dan Kejuruan (FTK) Universitas Pendidikan Ganesha mulai berdiri pada tahun 1990. Program studi awal yang ditawarkan adalah Pendidikan Kesejahteraan Keluarga di bawah Jurusan Ilmu Pendidikan.</t>
+  </si>
+  <si>
+    <t>Dekan Fakultas Teknik dan Kejuruan (FTK) Universitas Pendidikan Ganesha adalah Dr. Kadek Rihendra Dantes, S.T., M.T.</t>
+  </si>
+  <si>
+    <t>Kurikulum dikembangkan sesuai dengan visi, misi, tujuan, dan sasaran Undiksha yang berbasis kompetensi dan berorientasi Kerangka Kualifikasi Nasional Indonesia (KKNI).</t>
+  </si>
+  <si>
+    <t>Direktur Pascasarjana Universitas Pendidikan Ganesha adalah Prof. Dr. I Nyoman Jampel, M.Pd.</t>
+  </si>
+  <si>
+    <t>Anda dapat mengakses informasi mengenai tata cara pembayaran Uang Kuliah Tunggal (UKT) mahasiswa baru Universitas Pendidikan Ganesha dengan layanan BRI Virtual Account (BRIVA) melalui link berikut: https://undiksha.ac.id/prosedur-pembayaran-ukt-mahasiswa-baru-undiksha-dengan-layanan-bri-virtual-account-briva</t>
+  </si>
+  <si>
+    <t>Informasi lebih lanjut mengenai prosedur pembayaran Uang Kuliah Tunggal (UKT) mahasiswa baru Universitas Pendidikan Ganesha dengan layanan BRI Virtual Account (BRIVA) dapat ditemukan di situs resmi Undiksha melalui tautan berikut: https://undiksha.ac.id/prosedur-pembayaran-ukt-mahasiswa-baru-undiksha-dengan-layanan-bri-virtual-account-briva/.</t>
+  </si>
+  <si>
+    <t>Jadwal pendaftaran seleksi mahasiswa baru jalur mandiri (SMBJM) Universitas Pendidikan Ganesha untuk tahun 2025 akan diinformasikan segera. Untuk informasi lebih lanjut, Anda dapat mengunjungi situs resmi Undiksha atau mengikuti pengumuman resmi dari pihak universitas.</t>
+  </si>
+  <si>
+    <t>Biaya untuk mengikuti Seleksi Nasional Berdasarkan Tes (SNBT) adalah sebesar Rp200.000,00 (dua ratus ribu rupiah). Pembayaran dilakukan melalui mitra bank yang ditentukan.</t>
+  </si>
+  <si>
+    <t>Informasi lebih lanjut tentang UKM di Undiksha dapat diakses melalui laman https://undiksha.ac.id/kemahasiswaan/ukm/.</t>
+  </si>
+  <si>
+    <t>Kepala UPA TIK Universitas Pendidikan Ganesha saat ini adalah I Ketut Resika Arthana, S.T., M.Kom.</t>
+  </si>
+  <si>
+    <t>Motto Universitas Pendidikan Ganesha (Undiksha) adalah “dharmaning sajjana umerdhyaken widyaguna” yang berarti kewajiban orang bijaksana adalah mengembangkan ilmu pengetahuan dan pekerti.</t>
+  </si>
+  <si>
+    <t>Visi Universitas Pendidikan Ganesha (Undiksha) adalah menjadi Universitas Unggul Berlandaskan Falsafah Tri Hita Karana di Asia Pada Tahun 2045.</t>
+  </si>
+  <si>
+    <t>Rektor Universitas Pendidikan Ganesha saat ini adalah Prof. Dr. I Wayan Lasmawan, M.Pd.</t>
+  </si>
+  <si>
+    <t>Berikut informasi Kelulusan Peserta SMBJM di Undiksha (Universitas Pendidikan Ganesha):
 - Nomor Pendaftaran: 3242000006
 - Nama Siswa: KADEK YUNI SEDANI
 - Tanggal Lahir: 2005-11-30
@@ -366,92 +406,24 @@
 Selamat bergabung menjadi bagian dari Universitas Pendidikan Ganesha, KADEK YUNI SEDANI!</t>
   </si>
   <si>
-    <t>Salam Harmoni🙏
-Estimasi biaya kuliah adalah perkiraan biaya yang harus ditanggung oleh calon mahasiswa per semester jika mengikuti perkuliahan di Universitas Pendidikan Ganesha (Undiksha). Biaya ini mencakup berbagai komponen, seperti biaya pendidikan, biaya administrasi, dan biaya lainnya yang mungkin diperlukan selama proses perkuliahan. Estimasi ini penting untuk membantu calon mahasiswa merencanakan keuangan mereka selama menempuh pendidikan di Undiksha.</t>
-  </si>
-  <si>
-    <t>Apa itu Estimasi Biaya Kuliah?</t>
-  </si>
-  <si>
-    <t>Visi Fakultas Ekonomi</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Visi Fakultas Ekonomi (FE) Universitas Pendidikan Ganesha adalah "Menjadi Fakultas Unggul Berjiwa Wirausaha Berlandaskan Falsafah Tri Hita Karana di Asia Tahun 2045."</t>
-  </si>
-  <si>
-    <t>Kapan jadwal pendaftaran SMBJM?</t>
-  </si>
-  <si>
-    <t>Siapa nama Wakil Dekan I FE?</t>
-  </si>
-  <si>
-    <t>Siapa nama Dekan FIP?</t>
-  </si>
-  <si>
-    <t>Kapan FIP mulai berdiri dan apa jurusan awalnya?</t>
-  </si>
-  <si>
-    <t>Link informasi cara pembayaran UKT Mahasiswa Baru Undiksha dengan Layanan BRI Virtual Account (BRIVA)</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Informasi lebih lanjut mengenai prosedur pembayaran Uang Kuliah Tunggal (UKT) mahasiswa baru Universitas Pendidikan Ganesha dengan layanan BRI Virtual Account (BRIVA) dapat ditemukan di situs resmi Undiksha melalui tautan berikut: https://undiksha.ac.id/prosedur-pembayaran-ukt-mahasiswa-baru-undiksha-dengan-layanan-bri-virtual-account-briva/.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Anda dapat mengakses informasi mengenai tata cara pembayaran Uang Kuliah Tunggal (UKT) mahasiswa baru Universitas Pendidikan Ganesha dengan layanan BRI Virtual Account (BRIVA) melalui link berikut: https://undiksha.ac.id/prosedur-pembayaran-ukt-mahasiswa-baru-undiksha-dengan-layanan-bri-virtual-account-briva</t>
-  </si>
-  <si>
-    <t>Saya ingin lihat KTM, NIM saya 2115101014.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Berikut informasi Kartu Tanda Mahasiswa (KTM) Anda. 
+    <t>Berikut informasi Kartu Tanda Mahasiswa (KTM) Anda. 
 - NIM: 2115101014
 - Anda dapat mengunduh KTM Anda melalui tautan berikut: https://aka.undiksha.ac.id/api/ktm/generate/2115101014?token=NVNnV1dvQ2ZLRk10bFhQSFdpazBDTkZQaUpQQjl4SUg5YTJGOExSK3hzOVdFdWhGQjdGV1VtZWVRRWNCQXhHNGlzOVI0blUxM2F4cXBaQUFUWGVwcUdtcjZmM0lyNW1ibEtSRG9pbTBxOGpBamp5R3BlSU1yZ2dZd053aE1VeTFkQWJINEZWOUx5NFdTR1pjUnA3SFdqejBvOU42QmFURVlxeEEzY21BR0JVRUdmNHI2TmJ2UFlnYktNNXE3dmVLWWFOM0tDL0p1UnFGMnZoYzV5U1RJZmlSNjlyTkdGRG1tWFc1L3B4QUZHdGJ2SHVHSTJhWjdPQXBYZlNWMzVTSERSWXJ4T3ZEMmdUak9hdm5UT1hsT0M0Yi9pbG96ZUNGeEtmRDZKZlB2VitnUWNkZnpvcmxtMkFtcWJmcEo2TTYvRFpFVjB4MkNwdFdJVUVqVGtsNVdveFVPazhNQWtVeTlnNndPWkRpTEcyblRISDJWMm41T2pLQlFidjBpMDJJVS9DQnRHQXVzbWFVQkhrMm5tSHVHZnpRN3NDUlU4ZFlaRm1jWTV2eDFONTFjMTg0NEc1Z0tMdm9GS2c9.
 Silakan klik tautan tersebut untuk mengakses KTM Anda.</t>
   </si>
   <si>
-    <t>Salam Harmoni🙏
-Jadwal pendaftaran seleksi mahasiswa baru jalur mandiri (SMBJM) Universitas Pendidikan Ganesha untuk tahun 2025 akan diinformasikan segera. Untuk informasi lebih lanjut, Anda dapat mengunjungi situs resmi Undiksha atau mengikuti pengumuman resmi dari pihak universitas.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Nama Wakil Dekan I Fakultas Ekonomi (FE) Universitas Pendidikan Ganesha adalah Dr. Dra. Ni Made Suci, M.Si.</t>
-  </si>
-  <si>
-    <t>Siapa presiden indonesia sekarang?</t>
-  </si>
-  <si>
-    <t>Presiden</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Pertanyaan tersebut tidak relevan dengan konteks kampus Universitas Pendidikan Ganesha.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Fungsi utama Unit Kegiatan Mahasiswa (UKM) di Universitas Pendidikan Ganesha adalah sebagai wadah aktivitas kemahasiswaan yang bertujuan untuk:
-1. Mengembangkan Minat dan Bakat: UKM memberikan kesempatan bagi mahasiswa untuk mengembangkan minat dan bakat mereka dalam berbagai bidang, seperti seni, olahraga, akademik, dan lainnya.
-2. Meningkatkan Keahlian: Melalui berbagai kegiatan dan program yang diselenggarakan, UKM membantu mahasiswa untuk meningkatkan keahlian tertentu yang relevan dengan minat mereka.
-3. Membangun Kerjasama: UKM berfungsi sebagai partner organisasi kemahasiswaan intra kampus lainnya, seperti Badan Eksekutif Mahasiswa, untuk menciptakan sinergi dalam kegiatan kemahasiswaan.
-4. Mendorong Kemandirian: UKM bersifat otonom, yang memungkinkan mahasiswa untuk belajar mengelola organisasi dan kegiatan secara mandiri.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Informasi lebih lanjut tentang UKM di Undiksha dapat diakses melalui laman https://undiksha.ac.id/kemahasiswaan/ukm/</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Universitas Pendidikan Ganesha (Undiksha) memiliki akreditasi sebagai berikut:
-1. Terakreditasi A oleh Badan Akreditasi Nasional Perguruan Tinggi (BAN-PT).
-2. Terakreditasi internasional oleh AQAS (Agency for Quality Assurance in Higher Education) pada berbagai bidang studi.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Universitas Pendidikan Ganesha menyediakan berbagai jenis beasiswa bagi mahasiswa, antara lain:
-1. Bantuan Biaya Pendidikan (BKM)
+    <t>Anda dapat melihat KTM melalui SSO Undiksha atau dengan mengirimkan pesan yang berisi NIM (Nomor Induk Mahasiswa) yang valid. NIM yang valid dari Undiksha terdiri dari 10 digit angka. 
+Untuk mengirimkan pesan, gunakan format berikut:
+- KTM [NIM]
+Contoh penulisan pesan:
+- KTM 1234567890
+Silakan kirimkan NIM Anda untuk mendapatkan informasi lebih lanjut.</t>
+  </si>
+  <si>
+    <t>Pertanyaan tersebut tidak relevan dengan konteks kampus Universitas Pendidikan Ganesha.</t>
+  </si>
+  <si>
+    <t>1. Bantuan Biaya Pendidikan (BKM)
 2. Beasiswa Masuk Universitas (BMU)
 3. Beasiswa Tahun Pertama untuk mahasiswa baru
 4. Beasiswa dari Bank Indonesia
@@ -462,16 +434,12 @@
 9. Beasiswa dari berbagai Pemda</t>
   </si>
   <si>
-    <t>Salam Harmoni🙏
-Calon mahasiswa yang boleh ikut seleksi Mahasiswa Baru Jalur Mandiri (SMBJM) Universitas Pendidikan Ganesha adalah sebagai berikut:
-1. Calon mahasiswa yang BELUM mendapatkan tempat kuliah.
+    <t>1. Calon mahasiswa yang BELUM mendapatkan tempat kuliah.
 2. Calon mahasiswa yang TIDAK lolos pada seleksi SNMPTN atau SBMPTN.
 3. Calon mahasiswa yang SUDAH lolos pada seleksi SNMPTN atau SBMPTN tetapi hendak membatalkan pilihannya dan ingin memilih kampus atau Program Studi yang lain.</t>
   </si>
   <si>
-    <t>Salam Harmoni🙏
-Universitas Pendidikan Ganesha (Undiksha) memiliki berbagai fasilitas yang mendukung proses belajar mengajar, antara lain:
-1. Perpustakaan
+    <t>1. Perpustakaan
 2. UPT TIK (Unit Pelayanan Teknologi Informasi dan Komunikasi)
 3. Laboratorium
 4. Auditorium
@@ -487,14 +455,86 @@
 14. Unit pelayanan bahasa</t>
   </si>
   <si>
-    <t>Salam Harmoni🙏
-Fakultas Bahasa dan Seni (FBS) adalah salah satu fakultas di Universitas Pendidikan Ganesha (UNDIKSHA) yang bertujuan untuk menghasilkan sumber daya manusia berkualitas tinggi dalam bidang akademik dan vokasi, baik dalam kependidikan maupun non-kependidikan. FBS memiliki wawasan global yang berbasis pada kearifan lokal, humanis, berbudaya, dan peduli lingkungan.
-Visi Fakultas Bahasa dan Seni (FBS):
-FBS memiliki visi untuk menjadi fakultas yang unggul berlandaskan falsafah Tri Hita Karana dalam pengembangan sumber daya manusia di bidang bahasa dan seni di Asia pada tahun 2045.
-Misi Fakultas Bahasa dan Seni (FBS):
-1. Menyelenggarakan pendidikan dan pengajaran yang melahirkan sumber daya manusia yang kolaboratif, kompetitif, dan berkarakter dalam bidang bahasa dan seni.
-2. Menyelenggarakan penelitian yang kompetitif, kolaboratif, dan inovatif untuk pengembangan dan penerapan IPTEKS dalam bidang bahasa dan seni.
-3. Menyelenggarakan pengabdian kepada masyarakat yang akomodatif, kompetitif, kolaboratif, dan inovatif dalam bidang bahasa dan seni.
+    <t>1. Kecerdasan Intelektual: Pengembangan kemampuan berpikir kritis, analitis, dan kreatif.
+2. Kecerdasan Spiritual: Harmonisasi hubungan civitas akademika dengan Sang Pencipta.
+3. Kecerdasan Sosial: Harmonisasi hubungan antar sesama civitas akademika.
+4. Kecerdasan Ekologis: Harmonisasi hubungan civitas akademika dengan lingkungan.</t>
+  </si>
+  <si>
+    <t>1. Lulusan SMA/SMK/MA/Sederajat tahun 2023, 2024, dan 2025.
+2. Lulusan Paket C tahun 2023, 2024, dan 2025 dengan umur maksimal 25 tahun (per 1 Juli 2025).</t>
+  </si>
+  <si>
+    <t>1. Fleksibel: Proses seleksi dirancang untuk memberikan kemudahan bagi peserta dalam mengikuti ujian.
+2. Efisien: Mengutamakan penggunaan sumber daya secara optimal untuk mencapai hasil yang maksimal.
+3. Transparan: Proses seleksi dilakukan secara terbuka dan dapat dipertanggungjawabkan.
+4. Adil: Memberikan kesempatan yang sama bagi semua peserta tanpa diskriminasi.
+5. Larangan Berkonflik: Menghindari adanya konflik kepentingan dalam proses seleksi.
+6. Akuntabel: Setiap tahapan dan keputusan dalam proses seleksi dapat dipertanggungjawabkan.</t>
+  </si>
+  <si>
+    <t>1. Pengumuman Kuota Sekolah: 28 Desember 2024
+2. Masa Sanggah: 28 Desember 2024 – 17 Januari 2025
+3. Registrasi Akun SNPMB Sekolah: 6 – 31 Januari 2025
+4. Pengisian PDSS oleh Sekolah: 6 – 31 Januari 2025
+5. Registrasi Akun SNPMB Siswa: 13 Januari – 18 Februari 2025
+6. Pendaftaran SNBP: 4 – 18 Februari 2025
+7. Pengumuman Hasil SNBP: 18 Maret 2025
+8. Masa Unduh Kartu Peserta SNBP: 4 Februari – 30 April 2025</t>
+  </si>
+  <si>
+    <t>1. Merupakan siswa SMA/SMK/MA kelas terakhir pada tahun 2025 yang memiliki prestasi unggul.
+2. Memiliki NISN dan terdaftar di PDSS.
+3. Memiliki nilai rapor yang telah diisikan di PDSS sesuai dengan ketentuan.
+4. Memiliki prestasi akademik.
+5. Memenuhi persyaratan yang ditentukan oleh masing-masing PTN Akademik dan PTN Vokasi.</t>
+  </si>
+  <si>
+    <t>1. Registrasi Akun Siswa: 13 Januari – 27 Maret 2025
+2. Pendaftaran UTBK dan SNBT: 11 – 27 Maret 2025
+3. Pelaksanaan UTBK: 23 April – 03 Mei 2025
+4. Pengumuman Hasil SNBT: 28 Mei 2025
+5. Masa Unduh Sertifikat UTBK: 03 Juni – 31 Juli 2025
+Setiap tahapan UTBK-SNBT dibuka dan ditutup pada pukul 15.00 WIB.</t>
+  </si>
+  <si>
+    <t>1. Mengembangkan Minat dan Bakat: UKM memberikan kesempatan bagi mahasiswa untuk mengembangkan minat dan bakat mereka dalam berbagai bidang, seperti seni, olahraga, akademik, dan lainnya.
+2. Meningkatkan Keahlian: Melalui berbagai kegiatan dan program yang diselenggarakan, UKM membantu mahasiswa untuk meningkatkan keahlian tertentu yang relevan dengan minat mereka.
+3. Membangun Kerjasama: UKM berfungsi sebagai partner organisasi kemahasiswaan intra kampus lainnya, seperti Badan Eksekutif Mahasiswa, untuk menciptakan sinergi dalam kegiatan kemahasiswaan.
+4. Mendorong Kemandirian: UKM bersifat otonom, yang memungkinkan mahasiswa untuk belajar mengelola organisasi dan kegiatan secara mandiri.</t>
+  </si>
+  <si>
+    <t>Tugas utama dari UPA TIK Universitas Pendidikan Ganesha adalah melaksanakan pengembangan, pengelolaan, dan pelayanan teknologi informasi dan komunikasi serta pengelolaan sistem informasi dan jaringan. Secara lebih rinci, UPA TIK menyelenggarakan beberapa fungsi, yaitu:
+1. Penyusunan rencana, program, dan anggaran UPA.
+2. Pengembangan teknologi informasi dan komunik.
+3. Pengelolaan teknologi informasi dan komunikasi.
+4. Pemberian layanan di bidang teknologi informasi dan komunikasi.
+5. Pengembangan dan pengelolaan sistem informasi.
+6. Pengembangan dan pengelolaan jaringan.
+7. Pemeliharaan dan perbaikan jaringan.
+8. Pelaksanaan urusan tata usaha UPA.</t>
+  </si>
+  <si>
+    <t>1. Terakreditasi A oleh Badan Akreditasi Nasional Perguruan Tinggi (BAN-PT).
+2. Terakreditasi internasional oleh AQAS (Agency for Quality Assurance in Higher Education) pada berbagai bidang studi.</t>
+  </si>
+  <si>
+    <t>Untuk mengecek kelulusan Seleksi Mahasiswa Baru Jalur Mandiri (SMBJM), Anda dapat mengunjungi link berikut: https://penerimaan.undiksha.ac.id/smbjm/login
+Jika Anda ingin saya membantu, silakan kirimkan Nomor Pendaftaran dan Tanggal Lahir Anda. Berikut adalah format penulisan pesan yang perlu Anda gunakan:
+- Cek Kelulusan Nomor Pendaftaran [NO_PENDAFTARAN_10_DIGIT] Tanggal Lahir [YYYY-MM-DD]
+Contoh penulisan pesan yang benar adalah:
+- Cek Kelulusan Nomor Pendaftaran 1234567890 Tanggal Lahir 2001-01-31
+Silakan kirimkan informasi tersebut jika Anda memerlukan bantuan lebih lanjut.</t>
+  </si>
+  <si>
+    <t>1. Doktor Pendidikan Dasar
+2. Doktor Ilmu Pendidikan
+3. Doktor Pendidikan Bahasa
+4. Doktor Pendidikan Bahasa Inggris
+5. Doktor Teknologi Pendidikan</t>
+  </si>
+  <si>
+    <t>Fakultas Bahasa dan Seni (FBS) adalah salah satu fakultas di Universitas Pendidikan Ganesha (UNDIKSHA) yang bertujuan untuk menghasilkan sumber daya manusia berkualitas tinggi dalam bidang akademik dan vokasi, baik dalam kependidikan maupun non-kependidikan. FBS memiliki wawasan global yang berbasis pada kearifan lokal, humanis, berbudaya, dan peduli lingkungan. FBS memiliki visi untuk menjadi fakultas yang unggul berlandaskan falsafah Tri Hita Karana dalam pengembangan sumber daya manusia di bidang bahasa dan seni di Asia pada tahun 2045. Misi Fakultas Bahasa dan Seni (FBS) yaitu Menyelenggarakan pendidikan dan pengajaran yang melahirkan sumber daya manusia yang kolaboratif, kompetitif, dan berkarakter dalam bidang bahasa dan seni. Menyelenggarakan penelitian yang kompetitif, kolaboratif, dan inovatif untuk pengembangan dan penerapan IPTEKS dalam bidang bahasa dan seni. Menyelenggarakan pengabdian kepada masyarakat yang akomodatif, kompetitif, kolaboratif, dan inovatif dalam bidang bahasa dan seni.
 Pimpinan Fakultas Bahasa dan Seni (FBS):
 - Dekan: Drs. I Gede Nurjaya, M.Pd.
 - Wakil Dekan I: Dr. Ni Luh Putu Eka Sulistia Dewi, S.Pd. M.Pd.
@@ -504,116 +544,7 @@
 - Alamat: Jalan Ahmad Yani No. 67 Singaraja - Bali
 - Telepon: (0362) 21541
 - Email: fbs@undiksha.ac.id
-- Website:https://fbs.undiksha.ac.id
-Anda juga dapat melihat video profil Fakultas Bahasa dan Seni melalui link berikut https://youtu.be/DeLKu41DVn0.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Kurikulum Universitas Pendidikan Ganesha mengembangkan kecerdasan berdasarkan falsafah Tri Hita Karana yang meliputi empat jenis kecerdasan, yaitu:
-1. Kecerdasan Intelektual: Pengembangan kemampuan berpikir kritis, analitis, dan kreatif.
-2. Kecerdasan Spiritual: Harmonisasi hubungan civitas akademika dengan Sang Pencipta.
-3. Kecerdasan Sosial: Harmonisasi hubungan antar sesama civitas akademika.
-4. Kecerdasan Ekologis: Harmonisasi hubungan civitas akademika dengan lingkungan.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Fakultas Pascasarjana Universitas Pendidikan Ganesha menawarkan beberapa program doktoral, yaitu:
-- Doktor Pendidikan Dasar
-- Doktor Ilmu Pendidikan
-- Doktor Pendidikan Bahasa
-- Doktor Pendidikan Bahasa Inggris
-- Doktor Teknologi Pendidikan</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Kriteria peserta UTBK (Ujian Tulis Berbasis Komputer) mencakup:
-1. Lulusan SMA/SMK/MA/Sederajat tahun 2023, 2024, dan 2025.
-2. Lulusan Paket C tahun 2023, 2024, dan 2025 dengan umur maksimal 25 tahun (per 1 Juli 2025).</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Jadwal Seleksi Nasional Berdasarkan Prestasi (SNBP) 2025 adalah sebagai berikut:
-1. Pengumuman Kuota Sekolah: 28 Desember 2024
-2. Masa Sanggah: 28 Desember 2024 – 17 Januari 2025
-3. Registrasi Akun SNPMB Sekolah: 6 – 31 Januari 2025
-4. Pengisian PDSS oleh Sekolah: 6 – 31 Januari 2025
-5. Registrasi Akun SNPMB Siswa: 13 Januari – 18 Februari 2025
-6. Pendaftaran SNBP: 4 – 18 Februari 2025
-7. Pengumuman Hasil SNBP: 18 Maret 2025
-8. Masa Unduh Kartu Peserta SNBP: 4 Februari – 30 April 2025</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Syarat bagi siswa yang ingin mendaftar Seleksi Nasional Berdasarkan Prestasi (SNBP) adalah sebagai berikut:
-1. Merupakan siswa SMA/SMK/MA kelas terakhir pada tahun 2025 yang memiliki prestasi unggul.
-2. Memiliki NISN dan terdaftar di PDSS.
-3. Memiliki nilai rapor yang telah diisikan di PDSS sesuai dengan ketentuan.
-4. Memiliki prestasi akademik.
-5. Memenuhi persyaratan yang ditentukan oleh masing-masing PTN Akademik dan PTN Vokasi.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Jadwal Seleksi Nasional Berdasarkan Tes (SNBT) adalah sebagai berikut:
-1. Registrasi Akun Siswa: 13 Januari – 27 Maret 2025
-2. Pendaftaran UTBK dan SNBT: 11 – 27 Maret 2025
-3. Pelaksanaan UTBK: 23 April – 03 Mei 2025
-4. Pengumuman Hasil SNBT: 28 Mei 2025
-5. Masa Unduh Sertifikat UTBK: 03 Juni – 31 Juli 2025
-Setiap tahapan UTBK-SNBT dibuka dan ditutup pada pukul 15.00 WIB.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Tugas utama dari UPA TIK Universitas Pendidikan Ganesha adalah melaksanakan pengembangan, pengelolaan, dan pelayanan teknologi informasi dan komunikasi serta pengelolaan sistem informasi dan jaringan. Secara lebih rinci, UPA TIK menyelenggarakan beberapa fungsi, yaitu:
-1. Penyusunan rencana, program, dan anggaran UPA.
-2. Pengembangan teknologi informasi dan komunik.
-3. Pengelolaan teknologi informasi dan komunikasi.
-4. Pemberian layanan di bidang teknologi informasi dan komunikasi.
-5. Pengembangan dan pengelolaan sistem informasi.
-6. Pengembangan dan pengelolaan jaringan.
-7. Pemeliharaan dan perbaikan jaringan.
-8. Pelaksanaan urusan tata usaha UPA.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Untuk mengecek kelulusan Seleksi Mahasiswa Baru Jalur Mandiri (SMBJM), Anda dapat mengunjungi link berikut: https://penerimaan.undiksha.ac.id/smbjm/login
-Jika Anda ingin saya membantu, silakan kirimkan Nomor Pendaftaran dan Tanggal Lahir Anda. Berikut adalah format penulisan pesan yang perlu Anda gunakan:
-- Cek Kelulusan Nomor Pendaftaran [NO_PENDAFTARAN_10_DIGIT] Tanggal Lahir [YYYY-MM-DD]
-Contoh penulisan pesan yang benar adalah:
-- Cek Kelulusan Nomor Pendaftaran 1234567890 Tanggal Lahir 2001-01-31
-Silakan kirimkan informasi tersebut jika Anda memerlukan bantuan lebih lanjut.</t>
-  </si>
-  <si>
-    <t>Berapa daya tampung mahasiswa program studi ilmu komputer S1?</t>
-  </si>
-  <si>
-    <t>Kapan FK didirikan?</t>
-  </si>
-  <si>
-    <t>Apa visi dari FK?</t>
-  </si>
-  <si>
-    <t>Apa visi dari FMIPA?</t>
-  </si>
-  <si>
-    <t>Siapa Dekan FMIPA?</t>
-  </si>
-  <si>
-    <t>Apa visi dari FOK?</t>
-  </si>
-  <si>
-    <t>Kapan FTK mulai berdiri dan program studi awal apa yang ditawarkan?</t>
-  </si>
-  <si>
-    <t>Siapa Dekan FTK?</t>
-  </si>
-  <si>
-    <t>Apa fungsi utama UKM di Universitas Pendidikan Ganesha?</t>
-  </si>
-  <si>
-    <t>Apa tugas utama dari UPA TIK?</t>
-  </si>
-  <si>
-    <t>Siapa kepala UPA TIK saat ini?</t>
+- Website:https://fbs.undiksha.ac.id</t>
   </si>
 </sst>
 </file>
@@ -706,31 +637,12 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
         <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -810,6 +722,25 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -841,14 +772,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4DE5294B-EEB2-4C8B-A347-1013CA7914CB}" name="Table13" displayName="Table13" ref="A1:E51" totalsRowShown="0" headerRowDxfId="6" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4DE5294B-EEB2-4C8B-A347-1013CA7914CB}" name="Table13" displayName="Table13" ref="A1:E51" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E51" xr:uid="{CA3EBB52-0541-4D84-AA27-B220DF286A8D}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B3B35749-B31A-4D58-B0DB-CB4B8BEB47E8}" name="NO" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{DA99F610-8737-4D5B-8F7C-8BCC8F3621C7}" name="DOCUMENT" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{7AE09955-412F-48B8-827B-838B3CFB4C7E}" name="TARGET AGENT" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{850681BF-3655-4370-B3FA-48A29C2D0164}" name="QUESTION" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{FC230C4E-D812-43B5-9246-5219C076560C}" name="ANSWER" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{B3B35749-B31A-4D58-B0DB-CB4B8BEB47E8}" name="NO" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{DA99F610-8737-4D5B-8F7C-8BCC8F3621C7}" name="DOCUMENT" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{7AE09955-412F-48B8-827B-838B3CFB4C7E}" name="TARGET AGENT" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{850681BF-3655-4370-B3FA-48A29C2D0164}" name="QUESTION" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{FC230C4E-D812-43B5-9246-5219C076560C}" name="ANSWER" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1153,8 +1084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C236C3-56F3-4E8C-AE3B-EC9AC92EE935}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1184,7 +1115,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="180" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="135" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1195,13 +1126,13 @@
         <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1215,10 +1146,10 @@
         <v>4</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1229,13 +1160,13 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1246,13 +1177,13 @@
         <v>3</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1266,10 +1197,10 @@
         <v>7</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1280,13 +1211,13 @@
         <v>3</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="255" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="210" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1297,13 +1228,13 @@
         <v>3</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1317,10 +1248,10 @@
         <v>9</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1334,10 +1265,10 @@
         <v>11</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="390" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="255" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1351,10 +1282,10 @@
         <v>12</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1365,13 +1296,13 @@
         <v>3</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1382,13 +1313,13 @@
         <v>3</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1399,13 +1330,13 @@
         <v>3</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1416,13 +1347,13 @@
         <v>3</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1433,13 +1364,13 @@
         <v>3</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1450,13 +1381,13 @@
         <v>3</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1467,13 +1398,13 @@
         <v>3</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1484,13 +1415,13 @@
         <v>3</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1501,13 +1432,13 @@
         <v>3</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1518,13 +1449,13 @@
         <v>3</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>132</v>
+        <v>82</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1538,10 +1469,10 @@
         <v>36</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1552,13 +1483,13 @@
         <v>3</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>133</v>
+        <v>83</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1569,13 +1500,13 @@
         <v>3</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>134</v>
+        <v>84</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1586,13 +1517,13 @@
         <v>3</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>135</v>
+        <v>85</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1603,13 +1534,13 @@
         <v>3</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="105" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1623,10 +1554,10 @@
         <v>37</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1637,13 +1568,13 @@
         <v>3</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="120" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="75" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1654,13 +1585,13 @@
         <v>3</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1671,13 +1602,13 @@
         <v>3</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1691,10 +1622,10 @@
         <v>38</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="75" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1708,10 +1639,10 @@
         <v>53</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="150" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="90" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1725,10 +1656,10 @@
         <v>54</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1739,13 +1670,13 @@
         <v>3</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="165" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="120" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1759,10 +1690,10 @@
         <v>55</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="120" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="75" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1776,10 +1707,10 @@
         <v>56</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="150" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="90" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1793,10 +1724,10 @@
         <v>57</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1810,10 +1741,10 @@
         <v>58</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="105" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1824,13 +1755,13 @@
         <v>3</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1841,13 +1772,13 @@
         <v>3</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="180" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="150" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1858,13 +1789,13 @@
         <v>3</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>137</v>
+        <v>87</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1875,13 +1806,13 @@
         <v>3</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1895,10 +1826,10 @@
         <v>42</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="75" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1912,10 +1843,10 @@
         <v>39</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -1929,10 +1860,10 @@
         <v>40</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -1946,10 +1877,10 @@
         <v>41</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="165" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="135" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -1963,10 +1894,10 @@
         <v>28</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="165" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="135" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -1980,10 +1911,10 @@
         <v>30</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="180" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="150" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -1994,13 +1925,13 @@
         <v>32</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="165" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="135" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -2014,24 +1945,24 @@
         <v>34</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>111</v>
+        <v>77</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>